<commit_message>
[Receivable / Payable  Transactions] amount not show
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/cust_invoice.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/cust_invoice.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">{{fmt_date due_date}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{currency amount}}</t>
+    <t xml:space="preserve">{{currency due_amount}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{/each}}</t>
@@ -206,17 +206,17 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.0051020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>